<commit_message>
V 0.3 - Momento Fletor em ponto
</commit_message>
<xml_diff>
--- a/Valores.xlsx
+++ b/Valores.xlsx
@@ -404,13 +404,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>100</v>
+        <v>0.01</v>
       </c>
       <c r="B1" t="n">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="C1" t="n">
-        <v>10</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="2"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="A1:C12"/>
@@ -443,7 +443,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7</v>
+        <v>0.01</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -457,7 +457,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4"/>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10.01</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>
@@ -469,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
@@ -485,13 +493,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="n">
-        <v>100</v>
+        <v>0.01</v>
       </c>
       <c r="D1" t="n">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="E1" t="n">
-        <v>10</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="2">
@@ -502,16 +510,33 @@
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0.01</v>
       </c>
       <c r="D2" t="n">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D3" t="n">
+        <v>100000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>
@@ -523,7 +548,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
@@ -542,10 +567,24 @@
         <v>-10000</v>
       </c>
       <c r="D1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2"/>
+        <v>-16666.67</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-10000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>16666.67</v>
+      </c>
+    </row>
+    <row r="3"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>
@@ -574,18 +613,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="b">
         <v>1</v>
       </c>
       <c r="D1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -594,7 +633,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>